<commit_message>
optimize model and finish template format
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/Tab_51_rpt_PF_ADIExport.xlsx
+++ b/backend/reports/xlsx/Tab_51_rpt_PF_ADIExport.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robrien/work/gdx-agreements-tracker/backend/reports/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FDAF8F67-5B4F-6445-B87B-D989A07B4FC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B49A29-BD06-9C40-8374-D2DBA9FF66E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36920" yWindow="-21100" windowWidth="21600" windowHeight="37900" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="21100" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>{#r=d.report[i]}</t>
   </si>
@@ -50,16 +50,153 @@
     <t>{#date=d.date}</t>
   </si>
   <si>
-    <t>Project #</t>
-  </si>
-  <si>
-    <t>Project Name</t>
-  </si>
-  <si>
     <t>{#fy=d.fiscal_year}</t>
   </si>
   <si>
-    <t>Project ________ for {$fy} as of {$date}</t>
+    <t>Quarter</t>
+  </si>
+  <si>
+    <t>Portfolio</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Period</t>
+  </si>
+  <si>
+    <t>Preparer</t>
+  </si>
+  <si>
+    <t>Cl</t>
+  </si>
+  <si>
+    <t>Rsp</t>
+  </si>
+  <si>
+    <t>Srvc</t>
+  </si>
+  <si>
+    <t>STOB</t>
+  </si>
+  <si>
+    <t>Proj</t>
+  </si>
+  <si>
+    <t>Loc</t>
+  </si>
+  <si>
+    <t>Fut</t>
+  </si>
+  <si>
+    <t>Debit</t>
+  </si>
+  <si>
+    <t>Credit</t>
+  </si>
+  <si>
+    <t>Expense Authority 
+Name</t>
+  </si>
+  <si>
+    <t>Line 
+Description</t>
+  </si>
+  <si>
+    <t>Journal 
+Description</t>
+  </si>
+  <si>
+    <t>Journal 
+Name</t>
+  </si>
+  <si>
+    <t>Batch 
+Description</t>
+  </si>
+  <si>
+    <t>Batch 
+Name</t>
+  </si>
+  <si>
+    <t>Accounting 
+Date</t>
+  </si>
+  <si>
+    <t>Fiscal 
+Year</t>
+  </si>
+  <si>
+    <t>ADI Export for fiscal year {$fy} as of {$date}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{$r.fiscal_year} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{$r.quarter} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{$r.portfolio} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{$r.category} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{$r.accounting_date} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{$r.period} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{$r.batch_name} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{$r.batch_desc} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{$r.journal_name} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{$r.journal_desc} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{$r.preparer} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{$r.expense_authority_name} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{$r.cl} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{$r.rsp} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{$r.srvc} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{$r.stob} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{$r.proj} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{$r.loc} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{$r.fut} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{$r.debit} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{$r.credit} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{$r.line_desc} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{$r1.fiscal_year} </t>
   </si>
 </sst>
 </file>
@@ -69,7 +206,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -88,11 +225,6 @@
     </font>
     <font>
       <sz val="8.5"/>
-      <name val="BCSans-Regular"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
       <name val="BCSans-Regular"/>
     </font>
     <font>
@@ -121,12 +253,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor rgb="FFD9DADA"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -163,19 +295,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FFBFBFBF"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFBFBFBF"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFA5A5A5"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -201,49 +320,60 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -253,6 +383,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFD9DADA"/>
       <color rgb="FF003365"/>
       <color rgb="FFC5DAF1"/>
     </mruColors>
@@ -278,8 +409,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1561691</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>340181</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>680356</xdr:rowOff>
     </xdr:to>
@@ -623,115 +754,251 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:V12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I2" sqref="C2:I2"/>
+    <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="11.1640625" customWidth="1"/>
-    <col min="2" max="2" width="43.1640625" customWidth="1"/>
-    <col min="3" max="9" width="15.83203125" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" customWidth="1"/>
+    <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.33203125" customWidth="1"/>
+    <col min="11" max="11" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="9.5" customWidth="1"/>
+    <col min="17" max="19" width="5.6640625" customWidth="1"/>
+    <col min="20" max="21" width="9.83203125" customWidth="1"/>
+    <col min="22" max="22" width="55.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="57" customHeight="1" thickBot="1">
-      <c r="A1" s="15"/>
-      <c r="B1" s="15"/>
-      <c r="C1" s="16" t="s">
+    <row r="1" spans="1:22" s="1" customFormat="1" ht="57" customHeight="1" thickBot="1">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
+    </row>
+    <row r="2" spans="1:22" s="8" customFormat="1" ht="33" thickBot="1">
+      <c r="A2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
+      <c r="E2" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="P2" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q2" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="R2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="S2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="T2" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="U2" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="V2" s="11" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" ht="20" thickBot="1">
-      <c r="A2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
+    <row r="3" spans="1:22" s="2" customFormat="1" ht="20" thickBot="1">
+      <c r="A3" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="M3" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="N3" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="O3" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="P3" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q3" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="R3" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="S3" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="T3" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="U3" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="V3" s="17" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" ht="20" thickBot="1">
-      <c r="A3" s="5"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="10"/>
-    </row>
-    <row r="4" spans="1:9" s="2" customFormat="1" ht="20" thickBot="1">
-      <c r="A4" s="6"/>
-      <c r="B4" s="12"/>
+    <row r="4" spans="1:22" s="2" customFormat="1" ht="20" thickBot="1">
+      <c r="A4" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="16"/>
       <c r="C4" s="13"/>
       <c r="D4" s="13"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="10"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="15"/>
+      <c r="S4" s="15"/>
+      <c r="T4" s="15"/>
+      <c r="U4" s="15"/>
+      <c r="V4" s="18"/>
     </row>
-    <row r="5" spans="1:9" s="1" customFormat="1" ht="20" thickBot="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
+    <row r="7" spans="1:22">
+      <c r="A7" s="3" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="4" t="s">
-        <v>0</v>
+    <row r="8" spans="1:22">
+      <c r="A8" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="4" t="s">
-        <v>1</v>
+    <row r="9" spans="1:22">
+      <c r="A9" s="3" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="4" t="s">
-        <v>2</v>
-      </c>
+    <row r="10" spans="1:22">
+      <c r="A10" s="3"/>
     </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="4"/>
+    <row r="11" spans="1:22">
+      <c r="A11" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="4" t="s">
+    <row r="12" spans="1:22">
+      <c r="A12" s="3" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:I1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="5" scale="91" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="5" scale="59" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <headerFooter>
     <oddFooter>&amp;LTab_43_rpt_PF_RecoveryForecast
 &amp;C&amp;P of &amp;N&amp;R{$date}</oddFooter>

</xml_diff>